<commit_message>
Automate user order purchase flow
</commit_message>
<xml_diff>
--- a/tests/swaglab_testcases.xlsx
+++ b/tests/swaglab_testcases.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandeshaabeykoon/Downloads/GitHub/swaglabs-playwright-automation/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6D6C21-0484-2E4C-B9AB-3548F4FBBC42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1858AAED-B348-2D4D-A075-0202D51D2EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32920" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{B139ECD8-89FB-1D4C-B46F-8A62608ED91A}"/>
+    <workbookView xWindow="37720" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{B139ECD8-89FB-1D4C-B46F-8A62608ED91A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Plan" sheetId="3" r:id="rId1"/>
+    <sheet name="Business use cases" sheetId="3" r:id="rId1"/>
     <sheet name="Login Page" sheetId="1" r:id="rId2"/>
     <sheet name="Test Summary" sheetId="2" r:id="rId3"/>
   </sheets>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -118,6 +118,27 @@
   </si>
   <si>
     <t>Total test cases</t>
+  </si>
+  <si>
+    <t>Business Usecase ID</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Use case</t>
+  </si>
+  <si>
+    <t>Acceptance criteria</t>
+  </si>
+  <si>
+    <t>As a shopper, I want to login to the Swag Labs site, so I can view items and place orders.</t>
+  </si>
+  <si>
+    <t>As a shopper, I want to select and remove items, so I can upadate the cart with the items I wish to buy</t>
+  </si>
+  <si>
+    <t>As a shopper, I want to checkout the items in my shopping cart, so I can purchase the items selected</t>
   </si>
 </sst>
 </file>
@@ -219,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -231,6 +252,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -555,294 +582,354 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D86E7F6-4A8E-5C40-A811-74490D1616FD}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="47.6640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="42" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="B2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="B3" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="B4" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5172F61-CE0C-E543-AE9E-2983D1E5809A}">
-  <dimension ref="A2:F25"/>
+  <dimension ref="A2:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="15.1640625" customWidth="1"/>
-    <col min="3" max="3" width="27.83203125" customWidth="1"/>
-    <col min="4" max="4" width="27.6640625" customWidth="1"/>
-    <col min="5" max="5" width="43.33203125" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="27.83203125" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" customWidth="1"/>
+    <col min="6" max="6" width="43.33203125" customWidth="1"/>
+    <col min="7" max="7" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="7"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="9"/>
+      <c r="B4" s="4"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="9"/>
+      <c r="E4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="7"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="9"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="9"/>
+      <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="7"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="9"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="9"/>
+      <c r="E6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="8"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="10"/>
+      <c r="B7" s="5"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="1"/>
+      <c r="D7" s="10"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="8">
         <v>2</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="3" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="7"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="9"/>
+      <c r="B9" s="4"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="9"/>
+      <c r="E9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="7"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="9"/>
+      <c r="B10" s="4"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="9"/>
+      <c r="E10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
-      <c r="B11" s="8"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="10"/>
+      <c r="B11" s="5"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="1"/>
+      <c r="D11" s="10"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="8">
         <v>3</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="3" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="7"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="9"/>
+      <c r="B13" s="4"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="9"/>
+      <c r="E13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
-      <c r="B14" s="8"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="10"/>
+      <c r="B14" s="5"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="10"/>
+      <c r="E14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="D3:D7"/>
     <mergeCell ref="A3:A7"/>
-    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="D8:D11"/>
     <mergeCell ref="A8:A11"/>
-    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D14"/>
     <mergeCell ref="A12:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>